<commit_message>
Udate the files of the experiments
</commit_message>
<xml_diff>
--- a/Experiments' results/Experiments' results - the effect fo the number of nodes and edges on the ZKP of G3C.xlsx
+++ b/Experiments' results/Experiments' results - the effect fo the number of nodes and edges on the ZKP of G3C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BAR\Desktop\מצגת ואקסלים סופיים\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972BC33E-C4CF-43CB-B311-8E6FAE8D3CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C691C42E-AE5D-4394-A722-CF32BDC12475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -787,7 +787,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>כמות הזכרון של המוודאת כתלות במספר הקשתות</a:t>
+              <a:t>גודל הזכרון של המוודאת כתלות במספר הקשתות</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1137,7 +1137,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>כמות הזכרון של המוודאת (</a:t>
+                  <a:t>גודל הזכרון של המוודאת (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
@@ -2943,7 +2943,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="he-IL"/>
-              <a:t>כמות</a:t>
+              <a:t>אורך</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="he-IL" baseline="0"/>
@@ -3333,7 +3333,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="he-IL"/>
-                  <a:t>כמות</a:t>
+                  <a:t>אורך</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="he-IL" baseline="0"/>
@@ -3515,7 +3515,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>כמות התקשורת כתלות במספר הקשתות</a:t>
+              <a:t>אורך התקשורת כתלות במספר הקשתות</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3865,7 +3865,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>כמות התקשורת (</a:t>
+                  <a:t>אורך התקשורת (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
@@ -4049,7 +4049,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="he-IL"/>
-              <a:t>כמות הזכרון של המוכיח כתלות במספר הצמתים</a:t>
+              <a:t>גודל הזכרון של המוכיח כתלות במספר הצמתים</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4435,7 +4435,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="he-IL"/>
-                  <a:t>כמות</a:t>
+                  <a:t>גודל</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="he-IL" baseline="0"/>
@@ -4617,7 +4617,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>כמות הזכרון של המוודאת כתלות במספר הצמתים</a:t>
+              <a:t>גודל הזכרון של המוודאת כתלות במספר הצמתים</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5010,7 +5010,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>כמות הזכרון של המוודאת (</a:t>
+                  <a:t>גודל הזכרון של המוודאת (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
@@ -5201,7 +5201,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>כמות הזכרון של המוכיח כתלות במספר הקשתות</a:t>
+              <a:t>גודל הזכרון של המוכיח כתלות במספר הקשתות</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5551,7 +5551,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>כמות הזכרון של המוכיח (</a:t>
+                  <a:t>גודל הזכרון של המוכיח (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
@@ -11265,13 +11265,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>723372</xdr:colOff>
+      <xdr:colOff>347452</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>127438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1445759</xdr:colOff>
+      <xdr:colOff>1069839</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>8504</xdr:rowOff>
     </xdr:to>
@@ -11379,9 +11379,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>732305</xdr:colOff>
+      <xdr:colOff>999507</xdr:colOff>
       <xdr:row>136</xdr:row>
-      <xdr:rowOff>86846</xdr:rowOff>
+      <xdr:rowOff>79169</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11924,7 +11924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H118"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="77" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update the files of the experiments
</commit_message>
<xml_diff>
--- a/Experiments' results/Experiments' results - the effect fo the number of nodes and edges on the ZKP of G3C.xlsx
+++ b/Experiments' results/Experiments' results - the effect fo the number of nodes and edges on the ZKP of G3C.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BAR\Desktop\מצגת ואקסלים סופיים\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C691C42E-AE5D-4394-A722-CF32BDC12475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE46D002-FC08-4EC4-BB85-EA3988775ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>הגרף המלא</t>
   </si>
   <si>
     <t>מספר הצמתים (#)</t>
-  </si>
-  <si>
-    <t>כמות הנתונים שהועברה בתקשורת (MB)</t>
   </si>
   <si>
     <t>מספר הקשתות (#)</t>
@@ -48,19 +45,19 @@
     <t>זמן הריצה של המוודאת (s)</t>
   </si>
   <si>
-    <t>כמות התקשורת (MB)</t>
-  </si>
-  <si>
-    <t>השימוש בזיכרון של המוכיח (MB)</t>
-  </si>
-  <si>
-    <t>השימוש בזיכרון של המוודאת (MB)</t>
-  </si>
-  <si>
     <t>מדידות לבדיקת התלות במספר הקשתות:</t>
   </si>
   <si>
     <t>תוצאות הניסויים עבור המימוש של הוכחה באפס ידיעה ל-3 צביעות של גרף</t>
+  </si>
+  <si>
+    <t>מס' הביטים שעוברים בתקשורת (MB)</t>
+  </si>
+  <si>
+    <t>צריכת הזיכרון של המוכיח (MB)</t>
+  </si>
+  <si>
+    <t>צריכת הזיכרון של המוודאת (MB)</t>
   </si>
 </sst>
 </file>
@@ -787,7 +784,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>גודל הזכרון של המוודאת כתלות במספר הקשתות</a:t>
+              <a:t>צריכת הזיכרון של המוודאת כתלות במספר הקשתות</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1137,7 +1134,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>גודל הזכרון של המוודאת (</a:t>
+                  <a:t>צריכת הזיכרון של המוודאת (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
@@ -2943,11 +2940,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="he-IL"/>
-              <a:t>אורך</a:t>
+              <a:t>מס' הביטים שעוברים בתקשורת</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="he-IL" baseline="0"/>
-              <a:t> התקשורת כתלות במספר הצמתים</a:t>
+              <a:t> כתלות במספר הצמתים</a:t>
             </a:r>
             <a:endParaRPr lang="he-IL"/>
           </a:p>
@@ -3333,11 +3330,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="he-IL"/>
-                  <a:t>אורך</a:t>
+                  <a:t>מס' הביטים שעוברים בתקשורת</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="he-IL" baseline="0"/>
-                  <a:t> התקשורת (</a:t>
+                  <a:t> (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
@@ -3515,7 +3512,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>אורך התקשורת כתלות במספר הקשתות</a:t>
+              <a:t>מס' הביטים שעוברים בתקשורת כתלות במספר הקשתות</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3865,7 +3862,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>אורך התקשורת (</a:t>
+                  <a:t>מס' הביטים שעוברים בתקשורת (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
@@ -4049,7 +4046,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="he-IL"/>
-              <a:t>גודל הזכרון של המוכיח כתלות במספר הצמתים</a:t>
+              <a:t>צריכת הזיכרון של המוכיח כתלות במספר הצמתים</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4434,12 +4431,19 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="he-IL"/>
-                  <a:t>גודל</a:t>
+                  <a:rPr lang="he-IL" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>צריכת הזיכרון</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="he-IL" baseline="0"/>
-                  <a:t> הזכרון של המוכיח (</a:t>
+                  <a:t> של המוכיח (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
@@ -4617,7 +4621,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>גודל הזכרון של המוודאת כתלות במספר הצמתים</a:t>
+              <a:t>צריכת הזיכרון של המוודאת כתלות במספר הצמתים</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5002,6 +5006,17 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="he-IL" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>צריכת הזיכרון</a:t>
+                </a:r>
+                <a:r>
                   <a:rPr lang="he-IL" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
@@ -5010,7 +5025,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>גודל הזכרון של המוודאת (</a:t>
+                  <a:t> של המוודאת (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
@@ -5201,7 +5216,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>גודל הזכרון של המוכיח כתלות במספר הקשתות</a:t>
+              <a:t>צריכת הזיכרון של המוכיח כתלות במספר הקשתות</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5551,7 +5566,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>גודל הזכרון של המוכיח (</a:t>
+                  <a:t>צריכת הזיכרון של המוכיח (</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
@@ -11408,16 +11423,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1820883</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>96520</xdr:rowOff>
+      <xdr:rowOff>96519</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>108856</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11447,13 +11462,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>1734186</xdr:colOff>
       <xdr:row>119</xdr:row>
-      <xdr:rowOff>62865</xdr:rowOff>
+      <xdr:rowOff>62864</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>184729</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>150091</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11589,15 +11604,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>381001</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>121919</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
+      <xdr:colOff>1073729</xdr:colOff>
       <xdr:row>155</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>138545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11924,8 +11939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H118"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="77" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" zoomScale="82" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11942,12 +11957,12 @@
   <sheetData>
     <row r="2" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -11955,19 +11970,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="F5" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -12198,27 +12213,27 @@
     </row>
     <row r="105" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C106" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D106" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E106" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E106" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="F106" s="6" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H106" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>